<commit_message>
add export excel in users list
</commit_message>
<xml_diff>
--- a/src/media/exports/export-building-1.xlsx
+++ b/src/media/exports/export-building-1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <t>نام پروژه</t>
   </si>
@@ -48,9 +48,15 @@
     <t>test</t>
   </si>
   <si>
+    <t>ساختمان 1</t>
+  </si>
+  <si>
     <t>فعال</t>
   </si>
   <si>
+    <t>کرمان</t>
+  </si>
+  <si>
     <t>کد رهگیری</t>
   </si>
   <si>
@@ -87,22 +93,61 @@
     <t>ادرس عکس رسید</t>
   </si>
   <si>
-    <t>vlYQfOnfUh</t>
-  </si>
-  <si>
-    <t>تست تست|9130001123</t>
-  </si>
-  <si>
-    <t>2024-01-02 11:07:40</t>
-  </si>
-  <si>
-    <t>2024-01-10 00:00:00(40 دقیقه پیش)</t>
-  </si>
-  <si>
-    <t>تست</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:8000/media/images/users/9130001123/2024-01-02/RfZB0Gy7.JPG</t>
+    <t>m3VNu2Aflb</t>
+  </si>
+  <si>
+    <t>Fzl2 M2|9130009997</t>
+  </si>
+  <si>
+    <t>2023-10-18 13:16:08</t>
+  </si>
+  <si>
+    <t>2023-09-24 00:00:00(101  روز پیش)</t>
+  </si>
+  <si>
+    <t>awdwad</t>
+  </si>
+  <si>
+    <t>awd</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130009991/2023-10-18/KilPOgqb.png</t>
+  </si>
+  <si>
+    <t>wDA2H4NjXQ</t>
+  </si>
+  <si>
+    <t>test test|9130009999</t>
+  </si>
+  <si>
+    <t>2023-10-17 12:24:37</t>
+  </si>
+  <si>
+    <t>2023-10-05 00:00:00(90  روز پیش)</t>
+  </si>
+  <si>
+    <t>علی رضایی</t>
+  </si>
+  <si>
+    <t>سامان</t>
+  </si>
+  <si>
+    <t>WAWD</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130009999/2023-10-17/cohfPzI5.png</t>
+  </si>
+  <si>
+    <t>yGTOyj4lrj</t>
+  </si>
+  <si>
+    <t>2023-10-17 11:57:03</t>
+  </si>
+  <si>
+    <t>2023-10-03 00:00:00(92  روز پیش)</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130009999/2023-10-17/62MNmnro.png</t>
   </si>
   <si>
     <t>نام و نام خانوادگی</t>
@@ -117,10 +162,16 @@
     <t>امتیاز کل</t>
   </si>
   <si>
-    <t>تست تست</t>
-  </si>
-  <si>
-    <t>9130001123</t>
+    <t>Fzl2 M2</t>
+  </si>
+  <si>
+    <t>9130009997</t>
+  </si>
+  <si>
+    <t>test test</t>
+  </si>
+  <si>
+    <t>9130009999</t>
   </si>
 </sst>
 </file>
@@ -505,25 +556,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3">
-        <v>2000</v>
+        <v>850120000</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -533,7 +584,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -541,77 +592,146 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="L1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3">
-        <v>2000</v>
+        <v>120000</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4">
+        <v>750000000</v>
+      </c>
+      <c r="D4">
+        <v>114750</v>
+      </c>
+      <c r="E4">
+        <v>1.7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>100000000</v>
+      </c>
+      <c r="D5">
+        <v>9200</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
+        <v>37</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="L3" r:id="rId1"/>
+    <hyperlink ref="L4" r:id="rId2"/>
+    <hyperlink ref="L5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -619,7 +739,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -627,30 +747,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="C3">
-        <v>2000</v>
+        <v>120000</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>850000000</v>
+      </c>
+      <c r="D4">
+        <v>123950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update locale - add perm on all apps and ..
</commit_message>
<xml_diff>
--- a/src/media/exports/export-building-1.xlsx
+++ b/src/media/exports/export-building-1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="84">
   <si>
     <t>نام پروژه</t>
   </si>
@@ -93,16 +93,55 @@
     <t>ادرس عکس رسید</t>
   </si>
   <si>
+    <t>yGTOyj4lrj</t>
+  </si>
+  <si>
+    <t>test 2 test|9130009999</t>
+  </si>
+  <si>
+    <t>2023-10-17 11:57:03</t>
+  </si>
+  <si>
+    <t>2023-10-03 00:00:00(258  روز پیش)</t>
+  </si>
+  <si>
+    <t>علی رضایی</t>
+  </si>
+  <si>
+    <t>سامان 2</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130009999/2023-10-17/62MNmnro.png</t>
+  </si>
+  <si>
+    <t>wDA2H4NjXQ</t>
+  </si>
+  <si>
+    <t>2023-10-17 12:24:37</t>
+  </si>
+  <si>
+    <t>2023-10-05 00:00:00(256  روز پیش)</t>
+  </si>
+  <si>
+    <t>سامان</t>
+  </si>
+  <si>
+    <t>WAWD</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130009999/2023-10-17/cohfPzI5.png</t>
+  </si>
+  <si>
     <t>m3VNu2Aflb</t>
   </si>
   <si>
-    <t>Fzl2 M2|9130009997</t>
+    <t>Fzl20 M2|9130009997</t>
   </si>
   <si>
     <t>2023-10-18 13:16:08</t>
   </si>
   <si>
-    <t>2023-09-24 00:00:00(101  روز پیش)</t>
+    <t>2023-09-24 00:00:00(267  روز پیش)</t>
   </si>
   <si>
     <t>awdwad</t>
@@ -114,40 +153,91 @@
     <t>http://127.0.0.1:8000/media/images/users/9130009991/2023-10-18/KilPOgqb.png</t>
   </si>
   <si>
-    <t>wDA2H4NjXQ</t>
-  </si>
-  <si>
-    <t>test test|9130009999</t>
-  </si>
-  <si>
-    <t>2023-10-17 12:24:37</t>
-  </si>
-  <si>
-    <t>2023-10-05 00:00:00(90  روز پیش)</t>
-  </si>
-  <si>
-    <t>علی رضایی</t>
-  </si>
-  <si>
-    <t>سامان</t>
-  </si>
-  <si>
-    <t>WAWD</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:8000/media/images/users/9130009999/2023-10-17/cohfPzI5.png</t>
-  </si>
-  <si>
-    <t>yGTOyj4lrj</t>
-  </si>
-  <si>
-    <t>2023-10-17 11:57:03</t>
-  </si>
-  <si>
-    <t>2023-10-03 00:00:00(92  روز پیش)</t>
-  </si>
-  <si>
-    <t>http://127.0.0.1:8000/media/images/users/9130009999/2023-10-17/62MNmnro.png</t>
+    <t>XHKhdtPBnE</t>
+  </si>
+  <si>
+    <t>Test 234 test|9130001131</t>
+  </si>
+  <si>
+    <t>2024-06-13 07:05:41</t>
+  </si>
+  <si>
+    <t>2024-06-03 00:00:00(14  روز پیش)</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130001131/2024-06-13/aI083fGy.gif</t>
+  </si>
+  <si>
+    <t>tMi93SNDR2</t>
+  </si>
+  <si>
+    <t>2024-06-13 07:06:27</t>
+  </si>
+  <si>
+    <t>2024-06-19 00:00:00(29 دقیقه پیش)</t>
+  </si>
+  <si>
+    <t>awdwa</t>
+  </si>
+  <si>
+    <t>awdad</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130001131/2024-06-13/RrZeODQC.gif</t>
+  </si>
+  <si>
+    <t>Fcvh6nSXEs</t>
+  </si>
+  <si>
+    <t>2024-06-13 07:06:46</t>
+  </si>
+  <si>
+    <t>2024-06-12 00:00:00(5  روز پیش)</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130001131/2024-06-13/EZ58wEBC.gif</t>
+  </si>
+  <si>
+    <t>kuzIMh3iZv</t>
+  </si>
+  <si>
+    <t>2024-06-13 07:06:50</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130001131/2024-06-13/QGZj4YJL.gif</t>
+  </si>
+  <si>
+    <t>XdmbK9WeZt</t>
+  </si>
+  <si>
+    <t>2024-06-13 07:11:40</t>
+  </si>
+  <si>
+    <t>2024-06-13 00:00:00(4  روز پیش)</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130001131/2024-06-13/IbIDWkn8.png</t>
+  </si>
+  <si>
+    <t>kVHZh0lxBC</t>
+  </si>
+  <si>
+    <t>2024-06-13 07:52:36</t>
+  </si>
+  <si>
+    <t>2024-06-09 00:00:00(8  روز پیش)</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130001131/2024-06-13/jdKux9Hb.png</t>
+  </si>
+  <si>
+    <t>fOyRDX9m57</t>
+  </si>
+  <si>
+    <t>2024-06-13 08:01:15</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/media/images/users/9130001131/2024-06-13/ZwHsazUM.png</t>
   </si>
   <si>
     <t>نام و نام خانوادگی</t>
@@ -162,13 +252,19 @@
     <t>امتیاز کل</t>
   </si>
   <si>
-    <t>Fzl2 M2</t>
+    <t>Test 234 test</t>
+  </si>
+  <si>
+    <t>9130001131</t>
+  </si>
+  <si>
+    <t>Fzl20 M2</t>
   </si>
   <si>
     <t>9130009997</t>
   </si>
   <si>
-    <t>test test</t>
+    <t>test 2 test</t>
   </si>
   <si>
     <t>9130009999</t>
@@ -562,16 +658,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3">
-        <v>850120000</v>
+        <v>4092463346</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
@@ -584,7 +680,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -636,13 +732,13 @@
         <v>26</v>
       </c>
       <c r="C3">
-        <v>120000</v>
+        <v>100000000</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>64500</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="F3" t="s">
         <v>27</v>
@@ -665,66 +761,290 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>750000000</v>
       </c>
       <c r="D4">
-        <v>114750</v>
+        <v>326400</v>
       </c>
       <c r="E4">
         <v>1.7</v>
       </c>
       <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
         <v>34</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" t="s">
         <v>35</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>36</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="J4" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <v>120000</v>
+      </c>
+      <c r="D5">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5">
+      <c r="G5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6">
         <v>100000000</v>
       </c>
-      <c r="D5">
-        <v>9200</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="D6">
+        <v>1400</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" t="s">
         <v>42</v>
       </c>
-      <c r="H5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>43</v>
+      <c r="I6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <v>100000000</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>9</v>
+      </c>
+      <c r="I8" t="s">
+        <v>9</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10">
+        <v>123334</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11">
+        <v>3242340000</v>
+      </c>
+      <c r="D11">
+        <v>25938</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" t="s">
+        <v>69</v>
+      </c>
+      <c r="H11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>9</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -732,6 +1052,13 @@
     <hyperlink ref="L3" r:id="rId1"/>
     <hyperlink ref="L4" r:id="rId2"/>
     <hyperlink ref="L5" r:id="rId3"/>
+    <hyperlink ref="L6" r:id="rId4"/>
+    <hyperlink ref="L7" r:id="rId5"/>
+    <hyperlink ref="L8" r:id="rId6"/>
+    <hyperlink ref="L9" r:id="rId7"/>
+    <hyperlink ref="L10" r:id="rId8"/>
+    <hyperlink ref="L11" r:id="rId9"/>
+    <hyperlink ref="L12" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -739,7 +1066,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -747,44 +1074,58 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="C3">
-        <v>120000</v>
+        <v>3242463346</v>
       </c>
       <c r="D3">
-        <v>12</v>
+        <v>25940</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5">
         <v>850000000</v>
       </c>
-      <c r="D4">
-        <v>123950</v>
+      <c r="D5">
+        <v>390900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>